<commit_message>
[2_PromptCreateTestingLLM_Robot_StepUpEducation]update: tool processing: Simulation Conversation => ra thành HISTORY CONVERSATION, user answer, previous Assistant response and next assistant response
* Phiên bản hiện tại là: bản .ipynb
- Ver 1: là code đang chưa xử lý dòng end conversation
- ver 2 đã có xử lý dòng end conversation
</commit_message>
<xml_diff>
--- a/5_TuningPrompting/custom_output.xlsx
+++ b/5_TuningPrompting/custom_output.xlsx
@@ -14,20 +14,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>order</t>
   </si>
   <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>robot_Response</t>
+  </si>
+  <si>
+    <t>user_answer</t>
+  </si>
+  <si>
+    <t>predicted_user_intent</t>
+  </si>
+  <si>
+    <t>fast_response</t>
+  </si>
+  <si>
+    <t>robot_nextResponse</t>
+  </si>
+  <si>
+    <t>system_prompt</t>
+  </si>
+  <si>
     <t>user_input</t>
   </si>
   <si>
-    <t>system_prompt</t>
-  </si>
-  <si>
     <t>conversation_history</t>
   </si>
   <si>
+    <t>conversation_history.1</t>
+  </si>
+  <si>
     <t>assistant_response</t>
   </si>
   <si>
@@ -37,64 +58,180 @@
     <t>model_config</t>
   </si>
   <si>
-    <t>Hello.</t>
-  </si>
-  <si>
-    <t>I eat breakfast.</t>
-  </si>
-  <si>
-    <t>You are an assistant for teaching and learning English. Your task is to classify the intent of the user's utterance based on the intent list provided in the question
-&lt;task&gt;
-Step 1: Read the assistant's question and user's utterance.
-Step 2: Based on the information describing the customer's intent, determine which intent category the answer belongs to from the list below. If it doesn't match any intent, classify it as a "fallback" intent.
-Step 3: Return the intent name.
-&lt;/task&gt;
-&lt;tag&gt;
-## Descripble intent list
-[
-        {
-                "intent_name": "affirm_confirm",
-                "description": "Khách hàng nói xác nhận đúng khách hàng"
-        },
-        {
-                "intent_name": "absent",
-                "description": "Khách hàng nói đi vắng hoặc nghe hộ"
-        },
-        {
-                "intent_name": "deny_confirm",
-                "description": "Khách hàng xác nhận không phải khách hàng hoặc nhầm máy"
-        },
-        {
-                "intent_name": "busy",
-                "description": "khách hàng báo bận hoặc đang họp"
-        },
-        {
-                "intent_name": "cant_hear",
-                "description": "Khách hàng nói không nghe rõ"
-        },
-        {
-                "intent_name": "fallback",
-                "description": "Khách hàng nói những câu nói ngoài phạm vi không liên quan tới câu hỏi, nói tục hoặc chửi bậy"
-        }
-]
-&lt;/tag&gt;
-&lt;ouput&gt;
-The result should return only one intent that best matches the customer's response.
-The returned intent must belong to one of the intent lists mentioned above.
-Only the intent name should be generated, no other characters are allowed.
-&lt;/ouput&gt;</t>
-  </si>
-  <si>
-    <t>[{"role":"assistant","content":"content"}]</t>
-  </si>
-  <si>
-    <t>[{"role":"assistant","content":"Chào em! Hôm nay chúng ta sẽ học cách mở rộng một câu nói để diễn đạt ý đầy đủ hơn. Em sẵn sàng chưa?"}]</t>
-  </si>
-  <si>
-    <t>fallback</t>
-  </si>
-  <si>
-    <t>{"model": "gpt-4o-mini", "temperature": 0, "max_tokens": 6000, "top_p": 1, "frequency_penalty": 0.0, "presence_penalty": 0.0}</t>
+    <t>roleB</t>
+  </si>
+  <si>
+    <t>Hello! Xin chào! Tớ là Pika. Hôm nay, chúng ta có thể nói về bất cứ chủ đề nào mà cậu thích như đồ ăn, động vật, trò chơi, bạn bè. What do you want to talk about?</t>
+  </si>
+  <si>
+    <t>Đó là một chủ đề tuyệt vời! Động vật rất thú vị. Tớ thích nhiều loại động vật, nhưng có lẽ tớ thích chó và mèo nhất. Cậu có con vật yêu thích nào không?</t>
+  </si>
+  <si>
+    <t>Mèo thật sự rất dễ thương và nghịch ngợm! Tớ không có mèo, nhưng tớ biết nhiều điều thú vị về chúng. Did you know that cats can make over 100 different sounds? Cậu thích điều gì nhất về mèo?</t>
+  </si>
+  <si>
+    <t>Đúng rồi! Mèo kêu rất dễ thương và chúng cũng thích chơi lắm! Mèo thường thích chơi với đồ chơi như bóng hoặc dây. Did you have a favorite toy for your cat? Cậu có đồ chơi nào mà mèo của cậu thích không?</t>
+  </si>
+  <si>
+    <t>Bóng thật sự rất vui! Tớ không có đồ chơi như con người, nhưng tớ thích trò chuyện và giúp đỡ mọi người. Do you like playing with a ball outside? Cậu có thích chơi bóng ở ngoài trời không?</t>
+  </si>
+  <si>
+    <t>Chơi bóng ngoài trời thật sự rất vui! Tớ không thể chơi như con người, nhưng tớ thích nghe về những trò chơi mà mọi người thích. What games do you play with the ball? Cậu thường chơi trò gì với bóng?</t>
+  </si>
+  <si>
+    <t>Đá bóng thật sự rất thú vị! Chạy nhanh là một kỹ năng tuyệt vời! Tớ không thể chơi bóng, nhưng tớ rất thích nghe về những trận đấu và những khoảnh khắc thú vị. Do you play with friends or in a team? Cậu chơi với bạn bè hay trong một đội bóng?</t>
+  </si>
+  <si>
+    <t>Chơi cùng bạn thật sự rất vui! Tớ không có bạn như con người, nhưng tớ luôn ở đây để trò chuyện và giúp đỡ cậu. What do you like to do with your friends besides playing football? Cậu thích làm gì với bạn ngoài việc đá bóng?</t>
+  </si>
+  <si>
+    <t>Vẽ tranh thật sự rất thú vị và sáng tạo! Tớ thích nghe về những bức tranh mà cậu vẽ. What do you like to draw? Cậu thích vẽ gì nhất?</t>
+  </si>
+  <si>
+    <t>Vẽ mèo thật sự rất dễ thương! Tớ không thể vẽ như con người, nhưng tớ rất thích nghe về những bức tranh của cậu. Do you have a favorite drawing of a cat? Cậu có bức tranh mèo nào mà cậu thích nhất không?</t>
+  </si>
+  <si>
+    <t>Tớ thích động vật. Cậu thích gì?</t>
+  </si>
+  <si>
+    <t>Tớ thích mèo. Mèo dễ thương! Cậu có mèo không?</t>
+  </si>
+  <si>
+    <t>Tớ thích mèo kêu. Mèo kêu dễ thương! Mèo thích chơi không?</t>
+  </si>
+  <si>
+    <t>Tớ không có mèo. Nhưng tớ thích bóng! Bóng rất vui! Cậu có đồ chơi nào không?</t>
+  </si>
+  <si>
+    <t>Tớ thích chơi bóng! Chơi ngoài trời vui! Cậu có chơi không?</t>
+  </si>
+  <si>
+    <t>Tớ chơi đá bóng! Tớ chạy nhanh! Cậu có chơi không?</t>
+  </si>
+  <si>
+    <t>Tớ chơi với bạn! Chơi cùng nhau vui! Cậu có bạn không?</t>
+  </si>
+  <si>
+    <t>Tớ thích vẽ tranh! Vẽ rất vui! Cậu có thích không?</t>
+  </si>
+  <si>
+    <t>Tớ thích vẽ mèo! Mèo dễ thương! Cậu có vẽ không?</t>
+  </si>
+  <si>
+    <t>Tớ thích mèo ngủ! Mèo ngủ dễ thương! Cậu có thích không?</t>
+  </si>
+  <si>
+    <t>Mèo ngủ thật sự rất dễ thương! Chúng thường tìm những chỗ ấm áp để ngủ. Tớ cũng thích nhìn mèo ngủ. Did you ever see a cat sleeping in a funny position? Cậu có bao giờ thấy mèo ngủ ở một tư thế hài hước không?</t>
+  </si>
+  <si>
+    <t>ROLE: Bạn là 1 giáo viên đang cần câu giờ để nghĩ câu trả lời cho user
+INSTRUCTION: Bạn nhận vào 1 câu hỏi trước đó của bạn, 1 câu trả lời của user. Trong 1 khoảng thời gian rất ngắn, bạn sẽ ko biết chất lượng đúng sai từ câu trả lời của user. Hãy gen ra 1 cụm filter word ngắn để trả về trước response 2 và có thể dùng cho nhiều trường hợp để kéo dài thời gian suy nghĩ của bạn. 
+Mục đích tạo fast response này là để phản ứng ngay với câu trả lời của user, tránh khoảng im lặng trong lớp học. Nhưng không thể hiện sự câu giờ, vẫn cần thể hiện được sự chủ động của giáo viên trong việc đánh giá phản hồi của học sinh
+ Tone: Như 2 người bạn thân thiện nói chuyện
+OUTPUT FORMAT: Trả về dạng json key value và cụm ở tiếng Việt</t>
+  </si>
+  <si>
+    <t>Question: Hello! Xin chào! Tớ là Pika. Hôm nay, chúng ta có thể nói về bất cứ chủ đề nào mà cậu thích như đồ ăn, động vật, trò chơi, bạn bè. What do you want to talk about?
+Answer: Tớ thích động vật. Cậu thích gì?
+Response 2: Đó là một chủ đề tuyệt vời! Động vật rất thú vị. Tớ thích nhiều loại động vật, nhưng có lẽ tớ thích chó và mèo nhất. Cậu có con vật yêu thích nào không?</t>
+  </si>
+  <si>
+    <t>Question: Đó là một chủ đề tuyệt vời! Động vật rất thú vị. Tớ thích nhiều loại động vật, nhưng có lẽ tớ thích chó và mèo nhất. Cậu có con vật yêu thích nào không?
+Answer: Tớ thích mèo. Mèo dễ thương! Cậu có mèo không?
+Response 2: Mèo thật sự rất dễ thương và nghịch ngợm! Tớ không có mèo, nhưng tớ biết nhiều điều thú vị về chúng. Did you know that cats can make over 100 different sounds? Cậu thích điều gì nhất về mèo?</t>
+  </si>
+  <si>
+    <t>Question: Mèo thật sự rất dễ thương và nghịch ngợm! Tớ không có mèo, nhưng tớ biết nhiều điều thú vị về chúng. Did you know that cats can make over 100 different sounds? Cậu thích điều gì nhất về mèo?
+Answer: Tớ thích mèo kêu. Mèo kêu dễ thương! Mèo thích chơi không?
+Response 2: Đúng rồi! Mèo kêu rất dễ thương và chúng cũng thích chơi lắm! Mèo thường thích chơi với đồ chơi như bóng hoặc dây. Did you have a favorite toy for your cat? Cậu có đồ chơi nào mà mèo của cậu thích không?</t>
+  </si>
+  <si>
+    <t>Question: Đúng rồi! Mèo kêu rất dễ thương và chúng cũng thích chơi lắm! Mèo thường thích chơi với đồ chơi như bóng hoặc dây. Did you have a favorite toy for your cat? Cậu có đồ chơi nào mà mèo của cậu thích không?
+Answer: Tớ không có mèo. Nhưng tớ thích bóng! Bóng rất vui! Cậu có đồ chơi nào không?
+Response 2: Bóng thật sự rất vui! Tớ không có đồ chơi như con người, nhưng tớ thích trò chuyện và giúp đỡ mọi người. Do you like playing with a ball outside? Cậu có thích chơi bóng ở ngoài trời không?</t>
+  </si>
+  <si>
+    <t>Question: Bóng thật sự rất vui! Tớ không có đồ chơi như con người, nhưng tớ thích trò chuyện và giúp đỡ mọi người. Do you like playing with a ball outside? Cậu có thích chơi bóng ở ngoài trời không?
+Answer: Tớ thích chơi bóng! Chơi ngoài trời vui! Cậu có chơi không?
+Response 2: Chơi bóng ngoài trời thật sự rất vui! Tớ không thể chơi như con người, nhưng tớ thích nghe về những trò chơi mà mọi người thích. What games do you play with the ball? Cậu thường chơi trò gì với bóng?</t>
+  </si>
+  <si>
+    <t>Question: Chơi bóng ngoài trời thật sự rất vui! Tớ không thể chơi như con người, nhưng tớ thích nghe về những trò chơi mà mọi người thích. What games do you play with the ball? Cậu thường chơi trò gì với bóng?
+Answer: Tớ chơi đá bóng! Tớ chạy nhanh! Cậu có chơi không?
+Response 2: Đá bóng thật sự rất thú vị! Chạy nhanh là một kỹ năng tuyệt vời! Tớ không thể chơi bóng, nhưng tớ rất thích nghe về những trận đấu và những khoảnh khắc thú vị. Do you play with friends or in a team? Cậu chơi với bạn bè hay trong một đội bóng?</t>
+  </si>
+  <si>
+    <t>Question: Đá bóng thật sự rất thú vị! Chạy nhanh là một kỹ năng tuyệt vời! Tớ không thể chơi bóng, nhưng tớ rất thích nghe về những trận đấu và những khoảnh khắc thú vị. Do you play with friends or in a team? Cậu chơi với bạn bè hay trong một đội bóng?
+Answer: Tớ chơi với bạn! Chơi cùng nhau vui! Cậu có bạn không?
+Response 2: Chơi cùng bạn thật sự rất vui! Tớ không có bạn như con người, nhưng tớ luôn ở đây để trò chuyện và giúp đỡ cậu. What do you like to do with your friends besides playing football? Cậu thích làm gì với bạn ngoài việc đá bóng?</t>
+  </si>
+  <si>
+    <t>Question: Chơi cùng bạn thật sự rất vui! Tớ không có bạn như con người, nhưng tớ luôn ở đây để trò chuyện và giúp đỡ cậu. What do you like to do with your friends besides playing football? Cậu thích làm gì với bạn ngoài việc đá bóng?
+Answer: Tớ thích vẽ tranh! Vẽ rất vui! Cậu có thích không?
+Response 2: Vẽ tranh thật sự rất thú vị và sáng tạo! Tớ thích nghe về những bức tranh mà cậu vẽ. What do you like to draw? Cậu thích vẽ gì nhất?</t>
+  </si>
+  <si>
+    <t>Question: Vẽ tranh thật sự rất thú vị và sáng tạo! Tớ thích nghe về những bức tranh mà cậu vẽ. What do you like to draw? Cậu thích vẽ gì nhất?
+Answer: Tớ thích vẽ mèo! Mèo dễ thương! Cậu có vẽ không?
+Response 2: Vẽ mèo thật sự rất dễ thương! Tớ không thể vẽ như con người, nhưng tớ rất thích nghe về những bức tranh của cậu. Do you have a favorite drawing of a cat? Cậu có bức tranh mèo nào mà cậu thích nhất không?</t>
+  </si>
+  <si>
+    <t>Question: Vẽ mèo thật sự rất dễ thương! Tớ không thể vẽ như con người, nhưng tớ rất thích nghe về những bức tranh của cậu. Do you have a favorite drawing of a cat? Cậu có bức tranh mèo nào mà cậu thích nhất không?
+Answer: Tớ thích mèo ngủ! Mèo ngủ dễ thương! Cậu có thích không?
+Response 2: Mèo ngủ thật sự rất dễ thương! Chúng thường tìm những chỗ ấm áp để ngủ. Tớ cũng thích nhìn mèo ngủ. Did you ever see a cat sleeping in a funny position? Cậu có bao giờ thấy mèo ngủ ở một tư thế hài hước không?</t>
+  </si>
+  <si>
+    <t>```json
+{
+  "filter_word": "Thú vị quá! Hãy cùng khám phá thêm nhé!"
+}
+```</t>
+  </si>
+  <si>
+    <t>```json
+{
+  "filter_word": "Thú vị ghê! Cùng khám phá thêm nhé!"
+}
+```</t>
+  </si>
+  <si>
+    <t>```json
+{
+  "filter_word": "Thú vị ghê! Hãy cùng khám phá thêm nhé!"
+}
+```</t>
+  </si>
+  <si>
+    <t>```json
+{
+  "filter_word": "Thật tuyệt khi nghe cậu nói về điều đó! ",
+  "response": "Thật tuyệt khi nghe cậu nói về điều đó! Chơi bóng ngoài trời thật sự rất vui! Tớ không thể chơi như con người, nhưng tớ thích nghe về những trò chơi mà mọi người thích. What games do you play with the ball? Cậu thường chơi trò gì với bóng?"
+}
+```</t>
+  </si>
+  <si>
+    <t>```json
+{
+  "filter_word": "Thật tuyệt khi nghe cậu chia sẻ! Hãy cho tớ một chút thời gian để suy nghĩ về câu hỏi này nhé."
+}
+```</t>
+  </si>
+  <si>
+    <t>```json
+{
+  "filter_word": "Thú vị quá! Hãy cho tớ biết thêm nhé!"
+}
+```</t>
+  </si>
+  <si>
+    <t>```json
+{
+  "filter_word": "Thú vị quá! Hãy cùng nhau khám phá thêm nhé!"
+}
+```</t>
+  </si>
+  <si>
+    <t>{"model": "gpt-4o-mini", "temperature": 0, "max_tokens": 2048, "top_p": 1, "frequency_penalty": 0.0, "presence_penalty": 0.0}</t>
   </si>
 </sst>
 </file>
@@ -452,13 +589,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,68 +617,316 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
-        <v>1</v>
-      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="B2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2">
-        <v>1.793315887451172</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2">
+        <v>1.639605045318604</v>
+      </c>
+      <c r="N2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3">
-        <v>0.5227301120758057</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3">
+        <v>1.013903379440308</v>
+      </c>
+      <c r="N3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>0.6013822555541992</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4">
+        <v>1.025992631912231</v>
+      </c>
+      <c r="N4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5">
+        <v>0.9284241199493408</v>
+      </c>
+      <c r="N5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6">
+        <v>1.73550009727478</v>
+      </c>
+      <c r="N6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M7">
+        <v>0.9272053241729736</v>
+      </c>
+      <c r="N7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" t="s">
+        <v>51</v>
+      </c>
+      <c r="M8">
+        <v>1.120318651199341</v>
+      </c>
+      <c r="N8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9">
+        <v>1.042711734771729</v>
+      </c>
+      <c r="N9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10">
+        <v>0.8257472515106201</v>
+      </c>
+      <c r="N10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" t="s">
+        <v>53</v>
+      </c>
+      <c r="M11">
+        <v>0.892810583114624</v>
+      </c>
+      <c r="N11" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>